<commit_message>
div fixes + new tests
</commit_message>
<xml_diff>
--- a/docs/calculate_refinement_element_size.xlsx
+++ b/docs/calculate_refinement_element_size.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS2017_Projects\para-mesh-generator-v2\para-mesh-generator-v2\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS2017_Projects\para-mesh-generator-v2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3B6081-250D-44EB-A32C-E5A34E6C8B67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284D3B43-C6FF-4579-94B1-6A1C63171156}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{807FF2C9-8790-4A07-9358-3DAF00A8CCAD}"/>
   </bookViews>
@@ -174,8 +174,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -329,19 +329,19 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -494,7 +494,7 @@
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:xfrm rot="10800000">
+        <a:xfrm>
           <a:off x="7210425" y="400050"/>
           <a:ext cx="4324954" cy="4210638"/>
         </a:xfrm>
@@ -512,7 +512,7 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>34636</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="6696075" cy="7451079"/>
+    <xdr:ext cx="6696075" cy="10815077"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="7" name="TextBox 6">
@@ -527,7 +527,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7442489" y="5368636"/>
-          <a:ext cx="6696075" cy="7451079"/>
+          <a:ext cx="6696075" cy="10815077"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -615,6 +615,19 @@
         </a:p>
         <a:p>
           <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>PLATE:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
             <a:rPr lang="en-US" sz="1400">
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -745,13 +758,13 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>elL = L / (4 * (2^nRef - 1))</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400">
+            <a:t>elL = L / (3 * (2^nRef - 1))</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="1">
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:srgbClr val="FF0000"/>
             </a:solidFill>
             <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             <a:ea typeface="+mn-ea"/>
@@ -760,47 +773,60 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>-----------------------------------------------------</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>First row starts at distance = 0.0</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>-----------------------------------------------------</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1400">
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>CUBOID:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(FOR CUBOID, 3 will be 5!)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  L = 5elL * (2^nRef - 1)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>elL = L / (5 * (2^nRef - 1))</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="1">
             <a:solidFill>
-              <a:schemeClr val="accent6"/>
+              <a:srgbClr val="FFFF00"/>
             </a:solidFill>
             <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             <a:ea typeface="+mn-ea"/>
@@ -817,6 +843,58 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
+            <a:t>-----------------------------------------------------</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>First row starts at distance = 0.0</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>-----------------------------------------------------</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>PLATE:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>            nRefinements ---&gt;</a:t>
           </a:r>
         </a:p>
@@ -888,7 +966,18 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>24 + ...) + 2elL</a:t>
+            <a:t>24 + ...) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>+ 2elL</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1206,7 +1295,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>vs elL = L / (4 * (2^nRef - 1))</a:t>
+            <a:t>vs elL = L / (3 * (2^nRef - 1))</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1219,6 +1308,366 @@
             <a:ea typeface="+mn-ea"/>
             <a:cs typeface="+mn-cs"/>
           </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Cuboid:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> L =   elL * (</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(5-1)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> + 6 + </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>12</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> + 24 + ...)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> L =   elL * (6 + 12 + 24 + ...) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>+ 4elL</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> L =  6elL * sum(2^k) (k = 0 -&gt; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>nRefinements - 2</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>+ 4elL</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> L =  6elL * (2^(nRef</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>-1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>) - 1) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>+ 4elL</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> L =  6elL * 2^(nRef</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>-1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>) - 6elL </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>+ 4elL</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> L =  6elL * 2^(nRef</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>-1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>) - 2elL</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> L =   elL * (6*2^(nRef-1) - 2)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0"/>
+          <a:endParaRPr lang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>L = elL * (6 * 2^(nRef-1) - 2)   </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>vs   L =  5elL * (2^nRef - 1)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>elL =   L / (6 * 2^(nRef-1) - 2)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>   vs elL = L / (5 * (2^nRef - 1))</a:t>
+          </a:r>
         </a:p>
         <a:p>
           <a:pPr marL="0" indent="0"/>
@@ -1555,10 +2004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B369BE8-93C2-4D41-A427-B4A9B2E0F22A}">
-  <dimension ref="A2:X56"/>
+  <dimension ref="A2:X68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W48" sqref="W48:X56"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W75" sqref="W75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2520,6 +2969,9 @@
         <v>14</v>
       </c>
     </row>
+    <row r="68" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W68" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added more ref mesh height tests
</commit_message>
<xml_diff>
--- a/docs/calculate_refinement_element_size.xlsx
+++ b/docs/calculate_refinement_element_size.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS2017_Projects\para-mesh-generator-v2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284D3B43-C6FF-4579-94B1-6A1C63171156}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDFF31B-3067-4C77-A841-466BCABC4DB5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{807FF2C9-8790-4A07-9358-3DAF00A8CCAD}"/>
   </bookViews>
@@ -512,7 +512,7 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>34636</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="6696075" cy="10815077"/>
+    <xdr:ext cx="6921211" cy="12076576"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="7" name="TextBox 6">
@@ -527,7 +527,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7442489" y="5368636"/>
-          <a:ext cx="6696075" cy="10815077"/>
+          <a:ext cx="6921211" cy="12076576"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -794,8 +794,70 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>(FOR CUBOID, 3 will be 5!)</a:t>
-          </a:r>
+            <a:t>For Cuboid, 3 will be 5</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>            nRefinements ---&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> L =  elL * (5 + 10 + 20 + 40 + ...)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> L = 5elL * (1 + 2 +  4 +  8 + ...)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> L = 5elL * sum(2^k) (k = 0 -&gt; nRefinements - 1)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -1356,7 +1418,21 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> + 6 + </a:t>
+            <a:t> + 10 + 20 + 40 + ...)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> L =   elL * (10 + 20 + 40 + ...) </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1400" b="1">
@@ -1367,18 +1443,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>12</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> + 24 + ...)</a:t>
+            <a:t>+ 4elL</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1392,7 +1457,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> L =   elL * (6 + 12 + 24 + ...) </a:t>
+            <a:t> L = 10elL * sum(2^k) (k = 0 -&gt; </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1400" b="1">
@@ -1403,6 +1468,28 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
+            <a:t>nRefinements - 2</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>) </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>+ 4elL</a:t>
           </a:r>
         </a:p>
@@ -1417,7 +1504,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> L =  6elL * sum(2^k) (k = 0 -&gt; </a:t>
+            <a:t> L = 10elL * (2^(nRef</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1400" b="1">
@@ -1428,18 +1515,18 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>nRefinements - 2</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>) </a:t>
+            <a:t>-1</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>) - 1) </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1400" b="1">
@@ -1464,7 +1551,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> L =  6elL * (2^(nRef</a:t>
+            <a:t> L = 10elL * 2^(nRef</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1400" b="1">
@@ -1486,7 +1573,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>) - 1) </a:t>
+            <a:t>) - 10elL </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1400" b="1">
@@ -1511,7 +1598,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> L =  6elL * 2^(nRef</a:t>
+            <a:t> L = 10elL * 2^(nRef</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1400" b="1">
@@ -1533,18 +1620,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>) - 6elL </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1">
-              <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
-              </a:solidFill>
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>+ 4elL</a:t>
+            <a:t>) - 6elL</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1558,43 +1634,29 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> L =  6elL * 2^(nRef</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1">
-              <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
-              </a:solidFill>
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>-1</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>) - 2elL</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" indent="0"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="accent6"/>
-              </a:solidFill>
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> L =   elL * (6*2^(nRef-1) - 2)</a:t>
+            <a:t> L =   elL * (10*2^(nRef-1) -</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> 6</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1630,7 +1692,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>L = elL * (6 * 2^(nRef-1) - 2)   </a:t>
+            <a:t>L = elL * (10 * 2^(nRef-1) - 6)   </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
@@ -1655,7 +1717,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>elL =   L / (6 * 2^(nRef-1) - 2)</a:t>
+            <a:t>elL =   L / (10 * 2^(nRef-1) - 6)</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
@@ -2006,8 +2068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B369BE8-93C2-4D41-A427-B4A9B2E0F22A}">
   <dimension ref="A2:X68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W75" sqref="W75"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V64" sqref="V64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
clean up ref meshers with more functions
</commit_message>
<xml_diff>
--- a/docs/calculate_refinement_element_size.xlsx
+++ b/docs/calculate_refinement_element_size.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS2017_Projects\para-mesh-generator-v2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEDFF31B-3067-4C77-A841-466BCABC4DB5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A067593-5853-4F40-8F36-7B7CBB367FCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{807FF2C9-8790-4A07-9358-3DAF00A8CCAD}"/>
   </bookViews>
@@ -2068,8 +2068,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B369BE8-93C2-4D41-A427-B4A9B2E0F22A}">
   <dimension ref="A2:X68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V64" sqref="V64"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y77" sqref="Y77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
clean up plane mesher ref elements
</commit_message>
<xml_diff>
--- a/docs/calculate_refinement_element_size.xlsx
+++ b/docs/calculate_refinement_element_size.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VS2017_Projects\para-mesh-generator-v2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A067593-5853-4F40-8F36-7B7CBB367FCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6512E4DF-15D4-4F29-8120-B8C52A4025A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{807FF2C9-8790-4A07-9358-3DAF00A8CCAD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{807FF2C9-8790-4A07-9358-3DAF00A8CCAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>